<commit_message>
Changed Bios and Data
</commit_message>
<xml_diff>
--- a/src/data/summer20/bios_summer20.xlsx
+++ b/src/data/summer20/bios_summer20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{038F165E-A66C-1140-9374-D5EBC9F53BB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0031176D-5DCE-A547-B871-844D75990869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="293">
   <si>
     <t>Timestamp</t>
   </si>
@@ -887,6 +887,21 @@
   </si>
   <si>
     <t xml:space="preserve">Hello! My name is Uyen ("win") Sy and I initiated in my spring quarter of my freshman year. In my free time, I enjoy staying active outdoors and bullet journaling. A fun fact about myself is I have a family dog who is half German Shepherd and half Chihuahua. His name is Chase and he's a cutie! Ask me about anything you want at recruitment! </t>
+  </si>
+  <si>
+    <t>Cody</t>
+  </si>
+  <si>
+    <t>Enokida</t>
+  </si>
+  <si>
+    <t>Software Engineering Intern at Hack+ in Fremont, CA</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/codyenokida/</t>
+  </si>
+  <si>
+    <t>Hi hi! My name is Kota Cody Enokida and I initiated in my fall quarter of my freshman year. In my free time, I love to go outdoors, chill in my hammock, and surf. Ask me about music and my favorite tv shows!</t>
   </si>
 </sst>
 </file>
@@ -896,7 +911,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -910,6 +925,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -930,16 +951,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1255,13 +1279,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1914,7 +1938,7 @@
       <c r="L15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="4" t="s">
         <v>152</v>
       </c>
       <c r="P15" s="1" t="s">
@@ -2646,6 +2670,47 @@
       </c>
       <c r="P32" s="1" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
+        <v>44032.916488819443</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2682,6 +2747,7 @@
     <hyperlink ref="M30" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="M31" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="M32" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="M33" r:id="rId33" xr:uid="{7460DEAD-7672-144B-9FA0-A26749600BA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Bios and Chapter Stats
</commit_message>
<xml_diff>
--- a/src/data/summer20/bios_summer20.xlsx
+++ b/src/data/summer20/bios_summer20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer20/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Documents/UCI/Organizations/Delta_Sigma_Pi/Director_of_Technology/dspuci-website-gatsby/src/data/summer20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0031176D-5DCE-A547-B871-844D75990869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C1DD54-3A30-3E48-930D-36784A94C356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="292">
   <si>
     <t>Timestamp</t>
   </si>
@@ -437,9 +437,6 @@
   </si>
   <si>
     <t>Sunnyvale, CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business Adminstration </t>
   </si>
   <si>
     <t xml:space="preserve">Management Consulting </t>
@@ -679,9 +676,6 @@
     <t>kinda didnt follow the description template to a T so lmk if i should change anything !</t>
   </si>
   <si>
-    <t>Hello! My name is Lisa Deng, and I initiated in my fall quarter of my first year here at UCI. In my free time, I love working on projects, whether that's choreographing a dance, photoshopping my dad's face on fruit, or plotting how to take over the world. A fun fact about myself is that I've learned over 25 styles of dance. Ask me about anything above or my love for architecture at recruitment!</t>
-  </si>
-  <si>
     <t>Megha</t>
   </si>
   <si>
@@ -814,9 +808,6 @@
     <t>http://linkedin.com/in/ryanclau</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi! I’m Ryan and I’m a fourth-year Business Economics major, minoring one Management. I initiated in the Fall of 2019 with the Alpha Iota class. In my free time, I enjoy binging Netflix, eating, and hanging out with my dog. A fun fact: I used to compete doing olympic-style archery! Don’t be afraid to say hi at recruitment! </t>
-  </si>
-  <si>
     <t>Tiffany</t>
   </si>
   <si>
@@ -902,6 +893,12 @@
   </si>
   <si>
     <t>Hi hi! My name is Kota Cody Enokida and I initiated in my fall quarter of my freshman year. In my free time, I love to go outdoors, chill in my hammock, and surf. Ask me about music and my favorite tv shows!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi! I’m Ryan and I’m a fourth-year Business Economics major, minoring in Management. I initiated in the Fall of 2019 with the Alpha Iota class. In my free time, I enjoy binging Netflix, eating, and hanging out with my dog. A fun fact: I used to compete doing olympic-style archery! Don’t be afraid to say hi at recruitment! </t>
+  </si>
+  <si>
+    <t>Heyo! I’m Lisa, and I initiated in my fall quarter of my first year. In my free time, I love working on projects, whether that's watching all of Naruto &amp; Bojack Horseman in 3 months, photoshopping my dad's face on fruit, or plotting world domination. Fun fact: I’ve learned over 25 styles of dance (and counting!). Ask me about anything above or my love for architecture at recruitment :)</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1279,10 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P34" sqref="P34"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1877,28 +1874,28 @@
         <v>138</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M14" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1906,10 +1903,10 @@
         <v>44032.967619826391</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>109</v>
@@ -1924,25 +1921,25 @@
         <v>90</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="M15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1950,10 +1947,10 @@
         <v>44032.921501874996</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>100</v>
@@ -1962,31 +1959,31 @@
         <v>101</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="P16" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1994,10 +1991,10 @@
         <v>44039.744070462963</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>100</v>
@@ -2006,28 +2003,28 @@
         <v>101</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2035,10 +2032,10 @@
         <v>44032.963885023149</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>100</v>
@@ -2053,25 +2050,25 @@
         <v>90</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>95</v>
       </c>
       <c r="M18" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2079,10 +2076,10 @@
         <v>44033.684017349537</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
@@ -2097,25 +2094,25 @@
         <v>34</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M19" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2123,10 +2120,10 @@
         <v>44038.602950312503</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>61</v>
@@ -2141,25 +2138,25 @@
         <v>34</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M20" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2167,10 +2164,10 @@
         <v>44036.712978935189</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>100</v>
@@ -2182,25 +2179,25 @@
         <v>81</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="P21" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2208,10 +2205,10 @@
         <v>44036.762491817135</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
@@ -2220,7 +2217,7 @@
         <v>19</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>34</v>
@@ -2229,19 +2226,19 @@
         <v>44</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>133</v>
       </c>
       <c r="M22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2249,10 +2246,10 @@
         <v>44032.930597615741</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>100</v>
@@ -2261,31 +2258,31 @@
         <v>101</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I23" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M23" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="P23" s="1" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2293,10 +2290,10 @@
         <v>44041.898619988424</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
@@ -2305,31 +2302,31 @@
         <v>19</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>125</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2337,10 +2334,10 @@
         <v>44034.577034479167</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>18</v>
@@ -2355,28 +2352,28 @@
         <v>34</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="P25" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2384,10 +2381,10 @@
         <v>44034.038169652777</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>18</v>
@@ -2396,7 +2393,7 @@
         <v>32</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>53</v>
@@ -2405,19 +2402,19 @@
         <v>44</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2425,7 +2422,7 @@
         <v>44033.65097480324</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>17</v>
@@ -2443,22 +2440,22 @@
         <v>90</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2466,7 +2463,7 @@
         <v>44038.739518171293</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>70</v>
@@ -2478,16 +2475,16 @@
         <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>46</v>
@@ -2496,10 +2493,10 @@
         <v>38</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2507,10 +2504,10 @@
         <v>44037.478707314818</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>18</v>
@@ -2519,31 +2516,31 @@
         <v>32</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="L29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="P29" s="1" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2551,10 +2548,10 @@
         <v>44033.620099756939</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>18</v>
@@ -2569,22 +2566,22 @@
         <v>90</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2592,10 +2589,10 @@
         <v>44033.325196215279</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>109</v>
@@ -2604,31 +2601,31 @@
         <v>32</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="L31" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2636,10 +2633,10 @@
         <v>44032.916488819443</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
@@ -2648,28 +2645,28 @@
         <v>32</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>133</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2677,10 +2674,10 @@
         <v>44032.916488819443</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>100</v>
@@ -2698,19 +2695,19 @@
         <v>112</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Email List to Brothers page, Changed Careers Tab to show 2014-2020
</commit_message>
<xml_diff>
--- a/src/data/summer20/bios_summer20.xlsx
+++ b/src/data/summer20/bios_summer20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CD923D-5383-684C-84DA-9D92996F6107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ECC222-5B46-524B-953F-B8929E73B897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="345">
   <si>
     <t>Timestamp</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Any comments/questions about the website leave it here :)</t>
   </si>
   <si>
-    <t>Portfolio URL (optional)</t>
-  </si>
-  <si>
     <t>Bios</t>
   </si>
   <si>
@@ -497,9 +494,6 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/eugenemjeon</t>
-  </si>
-  <si>
-    <t>https://vsco.co/eugenej</t>
   </si>
   <si>
     <t xml:space="preserve">My name is Eugene Jeon and I initiated in Fall 2018 with the Alpha Eta Class! As a third-year, my free-time consists of listening to hi-fi audio, reading, and playing competitive FPS games. </t>
@@ -956,6 +950,114 @@
   </si>
   <si>
     <t>Hello hello! My name is Jocelyn and I initiated in the fall quarter of my freshman year. In my free time, I enjoy watching (and re-watching) cooking and dance videos, doing Blogilates, and exploring new views and eats. Fun fact, I used to have a pink streak in my hair! Ask me why I think leggings are superior to jeans or about my travel bucket list at recruitment – looking forward to meeting you!</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>briananderson@ucidsp.com</t>
+  </si>
+  <si>
+    <t>anshulbhanot@ucidsp.com</t>
+  </si>
+  <si>
+    <t>meghabhargava@ucidsp.com</t>
+  </si>
+  <si>
+    <t>meghancadigal@ucidsp.com</t>
+  </si>
+  <si>
+    <t>derekchang@ucidsp.com</t>
+  </si>
+  <si>
+    <t>lisadeng@ucidsp.com</t>
+  </si>
+  <si>
+    <t>codyenokida@ucidsp.com</t>
+  </si>
+  <si>
+    <t>aryanghanadan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>aimeehan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>gracehsiang@ucidsp.com</t>
+  </si>
+  <si>
+    <t>melaniehuang@ucidsp.com</t>
+  </si>
+  <si>
+    <t>tingtinghuang@ucidsp.com</t>
+  </si>
+  <si>
+    <t>eugenejeon@ucidsp.com</t>
+  </si>
+  <si>
+    <t>brandonkhong@ucidsp.com</t>
+  </si>
+  <si>
+    <t>akilakumar@ucidsp.com</t>
+  </si>
+  <si>
+    <t>jocelynkuo@ucidsp.com</t>
+  </si>
+  <si>
+    <t>ryanlau@ucidsp.com</t>
+  </si>
+  <si>
+    <t>edwardli@ucidsp.com</t>
+  </si>
+  <si>
+    <t>alanlim@ucidsp.com</t>
+  </si>
+  <si>
+    <t>julieluu@ucidsp.com</t>
+  </si>
+  <si>
+    <t>markmembrebe@ucidsp.com</t>
+  </si>
+  <si>
+    <t>gauravmohan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>sangoh@ucidsp.com</t>
+  </si>
+  <si>
+    <t>aishuparsuram@ucidsp.com</t>
+  </si>
+  <si>
+    <t>aayushshah@ucidsp.com</t>
+  </si>
+  <si>
+    <t>mohitshah@ucidsp.com</t>
+  </si>
+  <si>
+    <t>emilysu@ucidsp.com</t>
+  </si>
+  <si>
+    <t>uyensy@ucidsp.com</t>
+  </si>
+  <si>
+    <t>tiffanythan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>gracetill@ucidsp.com</t>
+  </si>
+  <si>
+    <t>ryanto@ucidsp.com</t>
+  </si>
+  <si>
+    <t>alinatu@ucidsp.com</t>
+  </si>
+  <si>
+    <t>patricktu@ucidsp.com</t>
+  </si>
+  <si>
+    <t>henrywang@ucidsp.com</t>
+  </si>
+  <si>
+    <t>ashleyyeh@ucidsp.com</t>
   </si>
 </sst>
 </file>
@@ -1353,10 +1455,10 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1418,10 +1520,10 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1429,43 +1531,46 @@
         <v>44038.591917731479</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1473,40 +1578,43 @@
         <v>44036.73588</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1514,40 +1622,43 @@
         <v>44032.94052340278</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1555,40 +1666,43 @@
         <v>44034.389569652776</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1596,40 +1710,43 @@
         <v>44038.779016828703</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1637,46 +1754,49 @@
         <v>44036.961599317132</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>77</v>
+      <c r="O7" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1684,40 +1804,43 @@
         <v>44036.738618784722</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1725,43 +1848,46 @@
         <v>44037.095246377314</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1769,40 +1895,43 @@
         <v>44038.840319421295</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="O10" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1810,40 +1939,43 @@
         <v>44042.649953854168</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="O11" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1851,40 +1983,43 @@
         <v>44034.473561817125</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="O12" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1892,40 +2027,43 @@
         <v>44039.494646099542</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="O13" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1933,43 +2071,46 @@
         <v>44037.674622523147</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1977,43 +2118,46 @@
         <v>44032.967619826391</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M15" s="4" t="s">
+      <c r="O15" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2021,43 +2165,43 @@
         <v>44032.921501874996</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M16" s="3" t="s">
+      <c r="O16" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2065,40 +2209,43 @@
         <v>44039.744070462963</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="O17" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2106,43 +2253,46 @@
         <v>44032.963885023149</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M18" s="3" t="s">
+      <c r="O18" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2150,43 +2300,46 @@
         <v>44033.684017349537</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="O19" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2194,43 +2347,46 @@
         <v>44038.602950312503</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M20" s="3" t="s">
+      <c r="O20" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2238,40 +2394,43 @@
         <v>44036.712978935189</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="M21" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>199</v>
+      <c r="O21" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2279,40 +2438,43 @@
         <v>44036.762491817135</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="K22" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="L22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="O22" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2320,43 +2482,46 @@
         <v>44032.930597615741</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="G23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>214</v>
+      <c r="O23" s="4" t="s">
+        <v>315</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2364,43 +2529,46 @@
         <v>44041.898619988424</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="O24" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2408,46 +2576,49 @@
         <v>44034.577034479167</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="I25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="K25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="M25" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="O25" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2455,40 +2626,43 @@
         <v>44034.038169652777</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="G26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="O26" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2496,40 +2670,43 @@
         <v>44033.65097480324</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="O27" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2537,40 +2714,43 @@
         <v>44038.739518171293</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="K28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="O28" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2578,43 +2758,46 @@
         <v>44037.478707314818</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="G29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="L29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>258</v>
+      <c r="O29" s="4" t="s">
+        <v>326</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2622,40 +2805,43 @@
         <v>44033.620099756939</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="L30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="O30" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2663,43 +2849,46 @@
         <v>44033.325196215279</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="O31" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2707,40 +2896,43 @@
         <v>44032.916488819443</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="G32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="L32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="O32" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="P32" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="P32" s="7" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2748,40 +2940,43 @@
         <v>44032.916488819443</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="K33" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="O33" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="P33" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2789,45 +2984,47 @@
         <v>44046.84337962963</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="G34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="I34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="L34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="N34" s="5"/>
+      <c r="O34" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="P34" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2835,40 +3032,43 @@
         <v>44046.84337962963</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>200</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M35" t="s">
         <v>299</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" t="s">
-        <v>202</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="M35" t="s">
-        <v>301</v>
+      <c r="O35" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2876,40 +3076,43 @@
         <v>44046.84337962963</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
         <v>300</v>
       </c>
-      <c r="D36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J36" t="s">
+        <v>301</v>
+      </c>
+      <c r="K36" t="s">
         <v>302</v>
       </c>
-      <c r="G36" t="s">
-        <v>89</v>
-      </c>
-      <c r="I36" t="s">
-        <v>255</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
+        <v>113</v>
+      </c>
+      <c r="M36" t="s">
         <v>303</v>
       </c>
-      <c r="K36" t="s">
+      <c r="O36" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="P36" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="L36" t="s">
-        <v>114</v>
-      </c>
-      <c r="M36" t="s">
-        <v>305</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2938,25 +3141,59 @@
     <hyperlink ref="M14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="M15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="M16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="O16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="M17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="M18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="M19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="M20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="M21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="M22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="M23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="M24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="M25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="M26" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="M27" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="M28" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="M29" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="M30" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="M31" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="M32" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="M33" r:id="rId33" xr:uid="{7460DEAD-7672-144B-9FA0-A26749600BA5}"/>
-    <hyperlink ref="M34" r:id="rId34" xr:uid="{B721E430-837E-DE4A-9FAC-154862F02F98}"/>
+    <hyperlink ref="M17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="M19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="M21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="M23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="M25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="M27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="M29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="M30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="M31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="M33" r:id="rId32" xr:uid="{7460DEAD-7672-144B-9FA0-A26749600BA5}"/>
+    <hyperlink ref="M34" r:id="rId33" xr:uid="{B721E430-837E-DE4A-9FAC-154862F02F98}"/>
+    <hyperlink ref="O2" r:id="rId34" xr:uid="{4E7413F3-EF96-3A4C-9DEC-A499D8F7B4A1}"/>
+    <hyperlink ref="O3" r:id="rId35" display="mailto:aimeehan@ucidsp.com" xr:uid="{57F36BDB-721F-AD43-B1A6-067B00C43376}"/>
+    <hyperlink ref="O4" r:id="rId36" display="mailto:aishuparsuram@ucidsp.com" xr:uid="{A57902F3-7415-4343-8470-2076368888C7}"/>
+    <hyperlink ref="O5" r:id="rId37" display="mailto:akilakumar@ucidsp.com" xr:uid="{BCD41697-9638-6E48-BA98-2B77FA284615}"/>
+    <hyperlink ref="O6" r:id="rId38" display="mailto:alanlim@ucidsp.com" xr:uid="{F444352E-7824-3344-A3A3-CA456DA39F4B}"/>
+    <hyperlink ref="O7" r:id="rId39" display="mailto:alinatu@ucidsp.com" xr:uid="{561E911C-63BF-3742-93E0-391EEA1F9A77}"/>
+    <hyperlink ref="O8" r:id="rId40" display="mailto:anshulbhanot@ucidsp.com" xr:uid="{63368282-7C63-044F-A398-4CB68522E450}"/>
+    <hyperlink ref="O9" r:id="rId41" display="mailto:aryanghanadan@ucidsp.com" xr:uid="{DB3E17A5-F497-FC4E-A1CC-25AC0AA7B1EE}"/>
+    <hyperlink ref="O10" r:id="rId42" display="mailto:ashleyyeh@ucidsp.com" xr:uid="{5AB94DB0-8A66-444F-A1CB-21553C250930}"/>
+    <hyperlink ref="O11" r:id="rId43" display="mailto:brandonkhong@ucidsp.com" xr:uid="{D6D816BE-551E-B74E-8A88-421C3C5D3C23}"/>
+    <hyperlink ref="O12" r:id="rId44" display="mailto:briananderson@ucidsp.com" xr:uid="{2443352C-A5C8-6E47-9F61-EBC58D1E288B}"/>
+    <hyperlink ref="O13" r:id="rId45" display="mailto:derekchang@ucidsp.com" xr:uid="{7F2099A7-0DAF-5A41-ADA4-E725107F393F}"/>
+    <hyperlink ref="O14" r:id="rId46" display="mailto:edwardli@ucidsp.com" xr:uid="{A7D4E02D-4ADA-DE46-BC79-A452DE9384FD}"/>
+    <hyperlink ref="O15" r:id="rId47" display="mailto:emilysu@ucidsp.com" xr:uid="{CB116AC5-CE14-B44D-8303-741AD26159A2}"/>
+    <hyperlink ref="O16" r:id="rId48" display="mailto:eugenejeon@ucidsp.com" xr:uid="{97E9BEC5-D636-E74F-ACF1-B77498381037}"/>
+    <hyperlink ref="O17" r:id="rId49" display="mailto:gauravmohan@ucidsp.com" xr:uid="{8705046E-8BDF-7440-BC5B-08C80FE5E5F8}"/>
+    <hyperlink ref="O18" r:id="rId50" display="mailto:gracehsiang@ucidsp.com" xr:uid="{69007E0A-3859-1443-B96B-16961CD14AC4}"/>
+    <hyperlink ref="O20" r:id="rId51" xr:uid="{4D365062-F470-0A44-BC1C-CAEF27CD6B0F}"/>
+    <hyperlink ref="O21" r:id="rId52" xr:uid="{02A6A1ED-9AD0-BB47-97D0-E4413625E052}"/>
+    <hyperlink ref="O22" r:id="rId53" xr:uid="{96A6123F-150C-6A4B-BC6E-329FD9317CCA}"/>
+    <hyperlink ref="O23" r:id="rId54" xr:uid="{28F547F5-5098-8541-BB94-70FDE134ED18}"/>
+    <hyperlink ref="O24" r:id="rId55" xr:uid="{55C15CBC-95BC-9D49-BEDF-CCEF87709BED}"/>
+    <hyperlink ref="O25" r:id="rId56" xr:uid="{80D76D2F-9EB2-4E4E-8489-9577479B05F7}"/>
+    <hyperlink ref="O26" r:id="rId57" xr:uid="{F23F1A81-8DAF-BA4D-9083-323AE556924C}"/>
+    <hyperlink ref="O27" r:id="rId58" xr:uid="{C7291C1B-A0C9-F94D-B88E-60D4DAC6A0D4}"/>
+    <hyperlink ref="O28" r:id="rId59" xr:uid="{B3E6EF5E-1B54-3149-87DF-6D014446644B}"/>
+    <hyperlink ref="O29" r:id="rId60" xr:uid="{7EBCB37D-E274-474C-93FD-C1F97E2548B4}"/>
+    <hyperlink ref="O30" r:id="rId61" xr:uid="{2F8E0385-D8B2-894D-AE00-352A0CB88E8E}"/>
+    <hyperlink ref="O31" r:id="rId62" xr:uid="{934C6746-B2C2-024C-9C7A-E1DB8FA4FD91}"/>
+    <hyperlink ref="O32" r:id="rId63" xr:uid="{74D43B9A-6D82-9A47-AB0E-E7DA3DF7CD7E}"/>
+    <hyperlink ref="O33" r:id="rId64" xr:uid="{AC0613A0-D546-5A45-91A0-B9C684B8E5A2}"/>
+    <hyperlink ref="O34" r:id="rId65" xr:uid="{7CE7FC15-DFF5-7241-96EF-E85BDB0E1AE6}"/>
+    <hyperlink ref="O35" r:id="rId66" xr:uid="{1CBA2270-57FC-4540-836E-01C0F21B7376}"/>
+    <hyperlink ref="O36" r:id="rId67" xr:uid="{9AB30801-61C1-6B49-86E3-75614E3C4409}"/>
+    <hyperlink ref="O19" r:id="rId68" xr:uid="{7EE3D629-CDEC-0843-8D37-E3E14688D160}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>